<commit_message>
fixing strain number and entering marker info for off by one errors
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0748.xlsx
+++ b/bioSample/bioSample_0748.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="32">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -82,13 +82,13 @@
     <t xml:space="preserve">G418</t>
   </si>
   <si>
+    <t xml:space="preserve">NAT</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDY1447</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_06352</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAT</t>
   </si>
   <si>
     <t xml:space="preserve">TDY1354</t>
@@ -130,6 +130,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -214,7 +215,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,7 +224,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="9.07"/>
@@ -383,6 +384,9 @@
       <c r="J5" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="K5" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -415,6 +419,9 @@
       <c r="J6" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="K6" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -447,6 +454,9 @@
       <c r="J7" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="K7" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -462,10 +472,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>16</v>
@@ -477,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,10 +504,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>16</v>
@@ -509,7 +519,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,10 +536,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>16</v>
@@ -541,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,7 +830,7 @@
         <v>3</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing problems with media, poly A protocol, marker
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0748.xlsx
+++ b/bioSample/bioSample_0748.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D7EE1A-A824-8A48-85B8-24E2029335E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4E77DC-B843-0942-B5CA-9A0009142FD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="37">
   <si>
     <t>harvestDate</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>marker_1</t>
-  </si>
-  <si>
-    <t>marker_2</t>
   </si>
   <si>
     <t>07.06.12</t>
@@ -500,7 +497,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -528,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -545,37 +542,35 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <v>90</v>
@@ -586,31 +581,31 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3">
         <v>90</v>
@@ -621,31 +616,31 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4">
         <v>90</v>
@@ -656,34 +651,34 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5">
         <v>90</v>
@@ -692,42 +687,39 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6">
         <v>90</v>
@@ -736,42 +728,39 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7">
         <v>90</v>
@@ -780,42 +769,39 @@
         <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8">
         <v>90</v>
@@ -824,39 +810,39 @@
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9">
         <v>90</v>
@@ -865,39 +851,39 @@
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10">
         <v>90</v>
@@ -906,39 +892,39 @@
         <v>3</v>
       </c>
       <c r="M10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11">
         <v>90</v>
@@ -947,39 +933,39 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12">
         <v>90</v>
@@ -988,39 +974,39 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13">
         <v>90</v>
@@ -1029,36 +1015,36 @@
         <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>16</v>
       </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14">
         <v>90</v>
@@ -1069,31 +1055,31 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
-        <v>17</v>
-      </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K15">
         <v>90</v>
@@ -1104,31 +1090,31 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16">
         <v>90</v>
@@ -1139,34 +1125,34 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17">
         <v>90</v>
@@ -1175,39 +1161,39 @@
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>30</v>
       </c>
-      <c r="F18" t="s">
-        <v>31</v>
-      </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18">
         <v>90</v>
@@ -1216,39 +1202,39 @@
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K19">
         <v>90</v>
@@ -1257,39 +1243,39 @@
         <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
         <v>32</v>
       </c>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20">
         <v>90</v>
@@ -1298,39 +1284,39 @@
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
         <v>32</v>
       </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21">
         <v>90</v>
@@ -1339,39 +1325,39 @@
         <v>2</v>
       </c>
       <c r="M21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
         <v>32</v>
       </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K22">
         <v>90</v>
@@ -1380,39 +1366,39 @@
         <v>3</v>
       </c>
       <c r="M22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" t="s">
-        <v>35</v>
-      </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K23">
         <v>90</v>
@@ -1421,39 +1407,39 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
         <v>34</v>
       </c>
-      <c r="F24" t="s">
-        <v>35</v>
-      </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K24">
         <v>90</v>
@@ -1462,39 +1448,39 @@
         <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" t="s">
-        <v>35</v>
-      </c>
       <c r="G25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K25">
         <v>90</v>
@@ -1503,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>